<commit_message>
complete up to rank 40
</commit_message>
<xml_diff>
--- a/us-mayoral-salaries.xlsx
+++ b/us-mayoral-salaries.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chrisgoodman/Dropbox/Data/Mayors/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chrisgoodman/Dropbox/Data/mayors-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EEFE5B0-90F8-244E-A8B5-591B3C4055FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D61F0B85-AC24-7346-8F35-1FC23B64E05E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11520" yWindow="1120" windowWidth="32180" windowHeight="18040" xr2:uid="{3052F3A6-D610-7D43-96F0-DD41B1A25444}"/>
+    <workbookView xWindow="0" yWindow="5860" windowWidth="27700" windowHeight="17540" xr2:uid="{3052F3A6-D610-7D43-96F0-DD41B1A25444}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="228">
   <si>
     <t>New York, New York</t>
   </si>
@@ -705,6 +705,18 @@
   </si>
   <si>
     <t>FY2017</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>FY2016</t>
+  </si>
+  <si>
+    <t>Check more on this</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Just confirmed via referendum </t>
   </si>
 </sst>
 </file>
@@ -1064,10 +1076,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF4CFCBD-9A88-7449-9EF0-DA14DD9A04C7}">
-  <dimension ref="A1:K101"/>
+  <dimension ref="A1:L101"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J42" sqref="J42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1082,7 +1094,7 @@
     <col min="10" max="10" width="12.5" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>105</v>
       </c>
@@ -1116,8 +1128,11 @@
       <c r="K1" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1152,7 +1167,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1187,7 +1202,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1222,7 +1237,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1257,7 +1272,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1292,7 +1307,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1327,7 +1342,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1362,7 +1377,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1397,7 +1412,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1432,7 +1447,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1467,7 +1482,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1502,7 +1517,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1537,7 +1552,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1572,7 +1587,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1607,7 +1622,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2020,6 +2035,12 @@
       <c r="I27" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="J27" s="4">
+        <v>185000</v>
+      </c>
+      <c r="K27" s="3" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28">
@@ -2049,6 +2070,12 @@
       <c r="I28" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="J28" s="4">
+        <v>24000</v>
+      </c>
+      <c r="K28" s="3" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29">
@@ -2078,6 +2105,12 @@
       <c r="I29" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="J29" s="4">
+        <v>126486.36</v>
+      </c>
+      <c r="K29" s="3">
+        <v>2019</v>
+      </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30">
@@ -2107,6 +2140,12 @@
       <c r="I30" s="3" t="s">
         <v>31</v>
       </c>
+      <c r="J30" s="4">
+        <v>143666</v>
+      </c>
+      <c r="K30" s="3" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31">
@@ -2136,6 +2175,12 @@
       <c r="I31" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="J31" s="4">
+        <v>144723.74</v>
+      </c>
+      <c r="K31" s="3">
+        <v>2018</v>
+      </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32">
@@ -2165,8 +2210,14 @@
       <c r="I32" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J32" s="4">
+        <v>147335.76</v>
+      </c>
+      <c r="K32" s="3" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
@@ -2194,8 +2245,17 @@
       <c r="I33" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J33" s="4">
+        <v>125000</v>
+      </c>
+      <c r="K33" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="L33" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
@@ -2223,8 +2283,17 @@
       <c r="I34" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J34" s="4">
+        <v>42000</v>
+      </c>
+      <c r="K34" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="L34" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
@@ -2252,8 +2321,14 @@
       <c r="I35" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J35" s="4">
+        <v>136900</v>
+      </c>
+      <c r="K35" s="3" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
@@ -2281,8 +2356,14 @@
       <c r="I36" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J36" s="4">
+        <v>130276</v>
+      </c>
+      <c r="K36" s="3">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
@@ -2310,8 +2391,14 @@
       <c r="I37" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J37" s="4">
+        <v>129391</v>
+      </c>
+      <c r="K37" s="3">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>37</v>
       </c>
@@ -2339,8 +2426,14 @@
       <c r="I38" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J38" s="4">
+        <v>141455</v>
+      </c>
+      <c r="K38" s="3" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>
@@ -2368,8 +2461,14 @@
       <c r="I39" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J39" s="4">
+        <v>73000</v>
+      </c>
+      <c r="K39" s="3" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>39</v>
       </c>
@@ -2397,8 +2496,14 @@
       <c r="I40" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J40" s="4">
+        <v>30000</v>
+      </c>
+      <c r="K40" s="3" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2426,8 +2531,14 @@
       <c r="I41" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J41" s="4">
+        <v>147500</v>
+      </c>
+      <c r="K41" s="3" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>41</v>
       </c>
@@ -2456,7 +2567,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>42</v>
       </c>
@@ -2485,7 +2596,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>43</v>
       </c>
@@ -2514,7 +2625,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>44</v>
       </c>
@@ -2543,7 +2654,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>45</v>
       </c>
@@ -2572,7 +2683,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>46</v>
       </c>
@@ -2601,7 +2712,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>47</v>
       </c>

</xml_diff>

<commit_message>
complete up to rank 50
</commit_message>
<xml_diff>
--- a/us-mayoral-salaries.xlsx
+++ b/us-mayoral-salaries.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chrisgoodman/Dropbox/Data/mayors-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D61F0B85-AC24-7346-8F35-1FC23B64E05E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4559D1BF-0FF7-9B46-B3E5-0308AE5ACD61}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="5860" windowWidth="27700" windowHeight="17540" xr2:uid="{3052F3A6-D610-7D43-96F0-DD41B1A25444}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="229">
   <si>
     <t>New York, New York</t>
   </si>
@@ -717,6 +717,9 @@
   </si>
   <si>
     <t xml:space="preserve">Just confirmed via referendum </t>
+  </si>
+  <si>
+    <t>In city charter as $250 per month</t>
   </si>
 </sst>
 </file>
@@ -1076,10 +1079,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF4CFCBD-9A88-7449-9EF0-DA14DD9A04C7}">
-  <dimension ref="A1:L101"/>
+  <dimension ref="A1:N101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J42" sqref="J42"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J52" sqref="J52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1092,6 +1095,7 @@
     <col min="6" max="6" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
@@ -2217,7 +2221,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
@@ -2255,7 +2259,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
@@ -2293,7 +2297,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
@@ -2328,7 +2332,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
@@ -2363,7 +2367,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
@@ -2398,7 +2402,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>37</v>
       </c>
@@ -2433,7 +2437,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>
@@ -2468,7 +2472,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>39</v>
       </c>
@@ -2503,7 +2507,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2538,7 +2542,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>41</v>
       </c>
@@ -2566,8 +2570,14 @@
       <c r="I42" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J42" s="4">
+        <v>114159</v>
+      </c>
+      <c r="K42" s="3" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>42</v>
       </c>
@@ -2595,8 +2605,16 @@
       <c r="I43" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J43" s="4">
+        <v>104358</v>
+      </c>
+      <c r="K43" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="M43" s="4"/>
+      <c r="N43" s="4"/>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>43</v>
       </c>
@@ -2624,8 +2642,14 @@
       <c r="I44" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J44" s="4">
+        <v>23720</v>
+      </c>
+      <c r="K44" s="3" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>44</v>
       </c>
@@ -2653,8 +2677,14 @@
       <c r="I45" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J45" s="4">
+        <v>97000</v>
+      </c>
+      <c r="K45" s="3" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>45</v>
       </c>
@@ -2682,8 +2712,14 @@
       <c r="I46" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J46" s="4">
+        <v>212000</v>
+      </c>
+      <c r="K46" s="3" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>46</v>
       </c>
@@ -2711,8 +2747,14 @@
       <c r="I47" s="3" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J47" s="4">
+        <v>126528</v>
+      </c>
+      <c r="K47" s="3" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>47</v>
       </c>
@@ -2740,8 +2782,14 @@
       <c r="I48" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J48" s="4">
+        <v>105000</v>
+      </c>
+      <c r="K48" s="3" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>48</v>
       </c>
@@ -2769,8 +2817,14 @@
       <c r="I49" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J49" s="4">
+        <v>140888.56</v>
+      </c>
+      <c r="K49" s="3" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>49</v>
       </c>
@@ -2798,8 +2852,14 @@
       <c r="I50" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J50" s="4">
+        <v>103560</v>
+      </c>
+      <c r="K50" s="3" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>50</v>
       </c>
@@ -2827,8 +2887,14 @@
       <c r="I51" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J51" s="4">
+        <v>3000</v>
+      </c>
+      <c r="L51" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>51</v>
       </c>
@@ -2857,7 +2923,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>52</v>
       </c>
@@ -2886,7 +2952,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>53</v>
       </c>
@@ -2915,7 +2981,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>54</v>
       </c>
@@ -2944,7 +3010,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>55</v>
       </c>
@@ -2973,7 +3039,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>56</v>
       </c>
@@ -3002,7 +3068,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>57</v>
       </c>
@@ -3031,7 +3097,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>58</v>
       </c>
@@ -3060,7 +3126,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>59</v>
       </c>
@@ -3089,7 +3155,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>60</v>
       </c>
@@ -3118,7 +3184,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>61</v>
       </c>
@@ -3147,7 +3213,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>62</v>
       </c>
@@ -3176,7 +3242,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>63</v>
       </c>
@@ -3205,7 +3271,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>64</v>
       </c>
@@ -3234,7 +3300,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>65</v>
       </c>
@@ -3262,8 +3328,14 @@
       <c r="I66" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J66" s="4">
+        <v>129000</v>
+      </c>
+      <c r="K66" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>66</v>
       </c>
@@ -3292,7 +3364,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>67</v>
       </c>
@@ -3321,7 +3393,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>68</v>
       </c>
@@ -3350,7 +3422,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>69</v>
       </c>
@@ -3379,7 +3451,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>70</v>
       </c>
@@ -3408,7 +3480,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>71</v>
       </c>
@@ -3437,7 +3509,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>72</v>
       </c>
@@ -3466,7 +3538,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>73</v>
       </c>
@@ -3495,7 +3567,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>74</v>
       </c>
@@ -3524,7 +3596,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>75</v>
       </c>
@@ -3553,7 +3625,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>76</v>
       </c>
@@ -3582,7 +3654,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>77</v>
       </c>
@@ -3611,7 +3683,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>78</v>
       </c>
@@ -3640,7 +3712,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>79</v>
       </c>

</xml_diff>